<commit_message>
completati perizia e chiusura
</commit_message>
<xml_diff>
--- a/closing/closing.xlsx
+++ b/closing/closing.xlsx
@@ -426,7 +426,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:C17"/>
+  <dimension ref="A1:C21"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -496,9 +496,14 @@
           <t>ACCERTAMENTI</t>
         </is>
       </c>
+      <c r="B4" s="2" t="inlineStr">
+        <is>
+          <t>Chiusura Post SelfCare</t>
+        </is>
+      </c>
       <c r="C4" s="2" t="inlineStr">
         <is>
-          <t>AvvioChiusura</t>
+          <t>VerificaChiusura</t>
         </is>
       </c>
     </row>
@@ -508,21 +513,26 @@
           <t>RIPARAZIONE</t>
         </is>
       </c>
+      <c r="B5" s="2" t="inlineStr">
+        <is>
+          <t>ChiusuraAvviata</t>
+        </is>
+      </c>
       <c r="C5" s="2" t="inlineStr">
         <is>
-          <t>AvvioChiusura</t>
+          <t>VerificaChiusura</t>
         </is>
       </c>
     </row>
     <row r="6">
       <c r="A6" s="2" t="inlineStr">
         <is>
-          <t>AvvioChiusura</t>
+          <t>ComunicazioneEsito</t>
         </is>
       </c>
       <c r="B6" s="2" t="inlineStr">
         <is>
-          <t>ChiusuraAvviata</t>
+          <t>AccordoRaggiunto-o-NonRichiesto</t>
         </is>
       </c>
       <c r="C6" s="2" t="inlineStr">
@@ -534,182 +544,255 @@
     <row r="7">
       <c r="A7" s="2" t="inlineStr">
         <is>
-          <t>VerificaChiusura</t>
+          <t>InvioEmailEsito</t>
         </is>
       </c>
       <c r="B7" s="2" t="inlineStr">
         <is>
-          <t>ChiusuraVerificata</t>
+          <t>EmailEsitoInviata</t>
         </is>
       </c>
       <c r="C7" s="2" t="inlineStr">
         <is>
-          <t>ChiusuraManuale</t>
+          <t>AttesaRicezioneAtto</t>
         </is>
       </c>
     </row>
     <row r="8">
       <c r="A8" s="2" t="inlineStr">
         <is>
-          <t>VerificaChiusura</t>
+          <t>InvioAtto</t>
         </is>
       </c>
       <c r="B8" s="2" t="inlineStr">
         <is>
-          <t>ChiusuraVerificata</t>
+          <t>AttoInviato</t>
         </is>
       </c>
       <c r="C8" s="2" t="inlineStr">
         <is>
-          <t>ChiusuraAutomatica</t>
+          <t>AttesaRicezioneAtto</t>
         </is>
       </c>
     </row>
     <row r="9">
       <c r="A9" s="2" t="inlineStr">
         <is>
-          <t>VerificaChiusura</t>
+          <t>AttesaRicezioneAtto</t>
         </is>
       </c>
       <c r="B9" s="2" t="inlineStr">
         <is>
-          <t>DatiObbligatoriMancanti</t>
+          <t>ConciliazioneAvviata</t>
         </is>
       </c>
       <c r="C9" s="2" t="inlineStr">
         <is>
-          <t>VerificaChiusura</t>
+          <t>ConciliazionePerizia</t>
         </is>
       </c>
     </row>
     <row r="10">
       <c r="A10" s="2" t="inlineStr">
         <is>
-          <t>VerificaChiusura</t>
+          <t>AttesaRicezioneAtto</t>
         </is>
       </c>
       <c r="B10" s="2" t="inlineStr">
         <is>
-          <t>PeriziaIncompleta</t>
+          <t>AttoFirmato</t>
         </is>
       </c>
       <c r="C10" s="2" t="inlineStr">
         <is>
-          <t>PERIZIA</t>
+          <t>VerificaChiusura</t>
         </is>
       </c>
     </row>
     <row r="11">
       <c r="A11" s="2" t="inlineStr">
         <is>
-          <t>GestioneRiapertura</t>
+          <t>AttesaRicezioneAtto</t>
         </is>
       </c>
       <c r="B11" s="2" t="inlineStr">
         <is>
-          <t>GestioneContestazione</t>
+          <t>ForzaturaChiusura</t>
         </is>
       </c>
       <c r="C11" s="2" t="inlineStr">
         <is>
-          <t>GestioneContestazione</t>
+          <t>VerificaChiusura</t>
         </is>
       </c>
     </row>
     <row r="12">
       <c r="A12" s="2" t="inlineStr">
         <is>
-          <t>GestioneRiapertura</t>
+          <t>VerificaChiusura</t>
         </is>
       </c>
       <c r="B12" s="2" t="inlineStr">
         <is>
-          <t>NonRiapertura</t>
+          <t>PeriziaIncompleta</t>
         </is>
       </c>
       <c r="C12" s="2" t="inlineStr">
         <is>
-          <t>SceltaManualeServizio</t>
+          <t>EsecuzionePerizia</t>
         </is>
       </c>
     </row>
     <row r="13">
       <c r="A13" s="2" t="inlineStr">
         <is>
-          <t>GestioneRiapertura</t>
+          <t>VerificaChiusura</t>
         </is>
       </c>
       <c r="B13" s="2" t="inlineStr">
         <is>
-          <t>PeriziaIntegrazione</t>
+          <t>DatiObbligatoriMancanti</t>
         </is>
       </c>
       <c r="C13" s="2" t="inlineStr">
         <is>
-          <t>PERIZIA</t>
+          <t>VerificaChiusura</t>
         </is>
       </c>
     </row>
     <row r="14">
       <c r="A14" s="2" t="inlineStr">
         <is>
-          <t>GestioneContestazione</t>
+          <t>VerificaChiusura</t>
         </is>
       </c>
       <c r="B14" s="2" t="inlineStr">
         <is>
-          <t>ContestazioneDaFinalizzare</t>
+          <t>ChiusuraVerificata</t>
         </is>
       </c>
       <c r="C14" s="2" t="inlineStr">
         <is>
-          <t>FinalizzaContestazione</t>
+          <t>ChiusuraAutomatica</t>
         </is>
       </c>
     </row>
     <row r="15">
       <c r="A15" s="2" t="inlineStr">
         <is>
-          <t>GestioneContestazione</t>
+          <t>VerificaChiusura</t>
         </is>
       </c>
       <c r="B15" s="2" t="inlineStr">
         <is>
-          <t>PeriziaContestazione</t>
+          <t>ChiusuraVerificata</t>
         </is>
       </c>
       <c r="C15" s="2" t="inlineStr">
         <is>
-          <t>PERIZIA</t>
+          <t>ChiusuraManuale</t>
         </is>
       </c>
     </row>
     <row r="16">
       <c r="A16" s="2" t="inlineStr">
         <is>
-          <t>FinalizzaContestazione</t>
+          <t>GestioneRiapertura</t>
         </is>
       </c>
       <c r="B16" s="2" t="inlineStr">
         <is>
-          <t>ChiusuraAvviata</t>
+          <t>PeriziaIntegrazione</t>
         </is>
       </c>
       <c r="C16" s="2" t="inlineStr">
         <is>
-          <t>AvvioChiusura</t>
+          <t>EsecuzionePerizia</t>
         </is>
       </c>
     </row>
     <row r="17">
       <c r="A17" s="2" t="inlineStr">
         <is>
-          <t>PERIZIA</t>
+          <t>GestioneRiapertura</t>
+        </is>
+      </c>
+      <c r="B17" s="2" t="inlineStr">
+        <is>
+          <t>GestioneContestazione</t>
         </is>
       </c>
       <c r="C17" s="2" t="inlineStr">
         <is>
-          <t>AvvioChiusura</t>
+          <t>GestioneContestazione</t>
+        </is>
+      </c>
+    </row>
+    <row r="18">
+      <c r="A18" s="2" t="inlineStr">
+        <is>
+          <t>GestioneRiapertura</t>
+        </is>
+      </c>
+      <c r="B18" s="2" t="inlineStr">
+        <is>
+          <t>NonRiapertura</t>
+        </is>
+      </c>
+      <c r="C18" s="2" t="inlineStr">
+        <is>
+          <t>SceltaManualeServizio</t>
+        </is>
+      </c>
+    </row>
+    <row r="19">
+      <c r="A19" s="2" t="inlineStr">
+        <is>
+          <t>GestioneContestazione</t>
+        </is>
+      </c>
+      <c r="B19" s="2" t="inlineStr">
+        <is>
+          <t>PeriziaContestazione</t>
+        </is>
+      </c>
+      <c r="C19" s="2" t="inlineStr">
+        <is>
+          <t>PeriziaContestazione</t>
+        </is>
+      </c>
+    </row>
+    <row r="20">
+      <c r="A20" s="2" t="inlineStr">
+        <is>
+          <t>GestioneContestazione</t>
+        </is>
+      </c>
+      <c r="B20" s="2" t="inlineStr">
+        <is>
+          <t>ContestazioneDaFinalizzare</t>
+        </is>
+      </c>
+      <c r="C20" s="2" t="inlineStr">
+        <is>
+          <t>FinalizzaContestazione</t>
+        </is>
+      </c>
+    </row>
+    <row r="21">
+      <c r="A21" s="2" t="inlineStr">
+        <is>
+          <t>FinalizzaContestazione</t>
+        </is>
+      </c>
+      <c r="B21" s="2" t="inlineStr">
+        <is>
+          <t>ChiusuraAvviata</t>
+        </is>
+      </c>
+      <c r="C21" s="2" t="inlineStr">
+        <is>
+          <t>VerificaChiusura</t>
         </is>
       </c>
     </row>

</xml_diff>